<commit_message>
GP1 - documentos corregidos
</commit_message>
<xml_diff>
--- a/GP1/tablas-de-ejercicios.xlsx
+++ b/GP1/tablas-de-ejercicios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UTN\2023\Sistema de Comunicaciones\Práctica\GP1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UTN\2023\Sistema de Comunicaciones\Práctica\COMUNICACIONES\GP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6022E5-65EE-454D-AFCD-33D1CB497376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A759D6-4521-44ED-BD31-36F36DC28CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{55E2434C-C16B-4684-96F0-BF38B1118731}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>A1</t>
   </si>
@@ -115,12 +115,6 @@
   </si>
   <si>
     <t>Cable Coaxil</t>
-  </si>
-  <si>
-    <t>11,75.10^-6</t>
-  </si>
-  <si>
-    <t>3,71.10^-3</t>
   </si>
   <si>
     <r>
@@ -140,7 +134,7 @@
   </si>
   <si>
     <r>
-      <t>0,4x10</t>
+      <t>18,05x10</t>
     </r>
     <r>
       <rPr>
@@ -156,7 +150,23 @@
   </si>
   <si>
     <r>
-      <t>54,77x10</t>
+      <t>31,62x10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10x10</t>
     </r>
     <r>
       <rPr>
@@ -171,8 +181,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>0,2x10</t>
+    <t>547,72x10-6</t>
+  </si>
+  <si>
+    <r>
+      <t>4,5x10</t>
     </r>
     <r>
       <rPr>
@@ -183,12 +196,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>-3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2x10</t>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4x10</t>
     </r>
     <r>
       <rPr>
@@ -204,7 +217,7 @@
   </si>
   <si>
     <r>
-      <t>1x10</t>
+      <t>400x10</t>
     </r>
     <r>
       <rPr>
@@ -216,86 +229,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>-6</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>244,95x10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>24,5x10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>18,05x10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>36,1x10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>36,1x10</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6</t>
     </r>
   </si>
 </sst>
@@ -384,11 +317,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,9 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D5BA81-ED02-4A0F-863D-4BA07F9584A9}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G10" sqref="A1:G10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -736,20 +667,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="C2" s="1">
+        <v>0.34639999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.8899999999999999E-2</v>
+      </c>
+      <c r="E2" s="6">
         <v>0.38</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -763,16 +694,16 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>75</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>300</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>600</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -786,13 +717,13 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>300</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>600</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -809,17 +740,17 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>28</v>
+      <c r="B5" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>17</v>
@@ -833,13 +764,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>17</v>
@@ -858,17 +789,17 @@
       <c r="B7" s="1">
         <v>100000</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>0.01</v>
       </c>
       <c r="D7" s="1">
-        <v>36100</v>
+        <v>4500</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>18</v>
@@ -882,10 +813,10 @@
         <v>-53.97</v>
       </c>
       <c r="C8" s="1">
-        <v>-6.99</v>
+        <v>-3.97</v>
       </c>
       <c r="D8" s="1">
-        <v>-30</v>
+        <v>-23.97</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>17</v>
@@ -905,10 +836,10 @@
         <v>-3.97</v>
       </c>
       <c r="C9" s="1">
-        <v>-26.99</v>
+        <v>-23.97</v>
       </c>
       <c r="D9" s="1">
-        <v>15.57</v>
+        <v>12.56</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>17</v>
@@ -924,20 +855,20 @@
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>50</v>
       </c>
       <c r="C10" s="1">
         <v>-20</v>
       </c>
       <c r="D10" s="1">
-        <v>45.57</v>
+        <v>36.53</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="1">
-        <v>75.569999999999993</v>
+        <v>66.53</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>16</v>
@@ -954,7 +885,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,11 +896,11 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
@@ -988,7 +919,7 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="4">
@@ -1008,7 +939,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="4">
         <v>65.16</v>
       </c>
@@ -1021,12 +952,12 @@
       <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="4">
         <v>18.14</v>
       </c>
@@ -1039,10 +970,10 @@
       <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="4">
         <v>48.14</v>
       </c>
@@ -1055,10 +986,10 @@
       <c r="E6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="4">
@@ -1077,71 +1008,71 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+    <row r="8" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
       <c r="B8" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D8" s="4">
-        <v>371.53</v>
+        <v>1000</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="4">
-        <v>-49.3</v>
+        <v>-45</v>
       </c>
       <c r="C9" s="4">
-        <v>-24.3</v>
+        <v>-20</v>
       </c>
       <c r="D9" s="4">
-        <v>25.7</v>
+        <v>30</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="4">
-        <v>-19.3</v>
+        <v>-15</v>
       </c>
       <c r="C10" s="4">
-        <v>5.7</v>
+        <v>10</v>
       </c>
       <c r="D10" s="4">
-        <v>55.7</v>
+        <v>60</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="4">
-        <v>29.24</v>
+        <v>33.729999999999997</v>
       </c>
       <c r="C11" s="4">
-        <v>54.32</v>
+        <v>58.75</v>
       </c>
       <c r="D11" s="4">
-        <v>104.44</v>
+        <v>108.75</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1152,5 +1083,6 @@
     <mergeCell ref="A7:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>